<commit_message>
new predicted prices and compared returns
</commit_message>
<xml_diff>
--- a/Code/Data/DAX30/Compared Returns/Auto Recurrence/input 125/DAX30_returns_compared_annual.xlsx
+++ b/Code/Data/DAX30/Compared Returns/Auto Recurrence/input 125/DAX30_returns_compared_annual.xlsx
@@ -501,13 +501,13 @@
         <v>0.131420741763922</v>
       </c>
       <c r="G2" t="n">
-        <v>0.11357929651269</v>
+        <v>0.1811440960505368</v>
       </c>
       <c r="H2" t="n">
-        <v>-13.57582145083424</v>
+        <v>37.8352409362713</v>
       </c>
       <c r="I2" t="n">
-        <v>14.33463665662848</v>
+        <v>3.460612640795781</v>
       </c>
     </row>
     <row r="3">
@@ -536,10 +536,10 @@
         <v>0.0890371962957979</v>
       </c>
       <c r="G3" t="n">
-        <v>0.1379368558418811</v>
+        <v>0.1533243439897147</v>
       </c>
       <c r="H3" t="n">
-        <v>54.92048444970072</v>
+        <v>72.20257416950002</v>
       </c>
       <c r="I3" t="inlineStr"/>
     </row>
@@ -569,10 +569,10 @@
         <v>-0.615343435918332</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.7043806186064799</v>
+        <v>-0.5924721202871878</v>
       </c>
       <c r="H4" t="n">
-        <v>14.46951043773951</v>
+        <v>3.71683750831132</v>
       </c>
       <c r="I4" t="inlineStr"/>
     </row>
@@ -602,10 +602,10 @@
         <v>-0.6105932447668134</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.5504698350129418</v>
+        <v>-0.6530015889596703</v>
       </c>
       <c r="H5" t="n">
-        <v>-9.846720426268863</v>
+        <v>-6.945432914026537</v>
       </c>
       <c r="I5" t="inlineStr"/>
     </row>
@@ -635,10 +635,10 @@
         <v>0.2461077835218171</v>
       </c>
       <c r="G6" t="n">
-        <v>0.1978923882237041</v>
+        <v>0.2042452669095475</v>
       </c>
       <c r="H6" t="n">
-        <v>-19.5911704246602</v>
+        <v>-17.00983041381889</v>
       </c>
       <c r="I6" t="inlineStr"/>
     </row>
@@ -668,10 +668,10 @@
         <v>0.1638219427486889</v>
       </c>
       <c r="G7" t="n">
-        <v>0.4080254058319217</v>
+        <v>0.3249686130804448</v>
       </c>
       <c r="H7" t="n">
-        <v>149.0663942728681</v>
+        <v>98.36696331880461</v>
       </c>
       <c r="I7" t="inlineStr"/>
     </row>
@@ -701,10 +701,10 @@
         <v>0.165308928384769</v>
       </c>
       <c r="G8" t="n">
-        <v>0.1137624084524876</v>
+        <v>0.1105988185832917</v>
       </c>
       <c r="H8" t="n">
-        <v>-31.18193338735037</v>
+        <v>-33.09567749065277</v>
       </c>
       <c r="I8" t="inlineStr"/>
     </row>
@@ -734,10 +734,10 @@
         <v>0.1950925388973966</v>
       </c>
       <c r="G9" t="n">
-        <v>0.1943353395306265</v>
+        <v>0.2142664248883905</v>
       </c>
       <c r="H9" t="n">
-        <v>-0.3881231804401951</v>
+        <v>9.828098039709177</v>
       </c>
       <c r="I9" t="inlineStr"/>
     </row>
@@ -767,10 +767,10 @@
         <v>-0.05714634763265068</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.07899670394197629</v>
+        <v>-0.1245222012327999</v>
       </c>
       <c r="H10" t="n">
-        <v>38.23578796283625</v>
+        <v>-117.9005420140865</v>
       </c>
       <c r="I10" t="inlineStr"/>
     </row>
@@ -800,10 +800,10 @@
         <v>-0.1187683230189159</v>
       </c>
       <c r="G11" t="n">
-        <v>-0.1073105656178869</v>
+        <v>-0.1265913573149279</v>
       </c>
       <c r="H11" t="n">
-        <v>-9.647149264879454</v>
+        <v>-6.58680201686947</v>
       </c>
       <c r="I11" t="inlineStr"/>
     </row>
@@ -833,10 +833,10 @@
         <v>0.1590292857940055</v>
       </c>
       <c r="G12" t="n">
-        <v>0.2137937753069803</v>
+        <v>0.1850839586032318</v>
       </c>
       <c r="H12" t="n">
-        <v>34.43673235375815</v>
+        <v>16.38356902575514</v>
       </c>
       <c r="I12" t="inlineStr"/>
     </row>
@@ -866,10 +866,10 @@
         <v>0.2056617473000462</v>
       </c>
       <c r="G13" t="n">
-        <v>0.2281620220954408</v>
+        <v>0.2067866592343471</v>
       </c>
       <c r="H13" t="n">
-        <v>10.9404277123875</v>
+        <v>0.5469718842073983</v>
       </c>
       <c r="I13" t="inlineStr"/>
     </row>
@@ -899,10 +899,10 @@
         <v>0.1893730763108184</v>
       </c>
       <c r="G14" t="n">
-        <v>0.2194054611433626</v>
+        <v>0.1750487029835016</v>
       </c>
       <c r="H14" t="n">
-        <v>15.85884615575024</v>
+        <v>-7.564102356243183</v>
       </c>
       <c r="I14" t="inlineStr"/>
     </row>
@@ -932,10 +932,10 @@
         <v>0.2499054176184599</v>
       </c>
       <c r="G15" t="n">
-        <v>0.2269687900091851</v>
+        <v>0.2833445696460045</v>
       </c>
       <c r="H15" t="n">
-        <v>-9.178123398786429</v>
+        <v>13.38072313366068</v>
       </c>
       <c r="I15" t="inlineStr"/>
     </row>
@@ -965,10 +965,10 @@
         <v>0.03648024689456582</v>
       </c>
       <c r="G16" t="n">
-        <v>0.003647765023152569</v>
+        <v>0.05123395413793603</v>
       </c>
       <c r="H16" t="n">
-        <v>-90.00071179974402</v>
+        <v>40.44300271873422</v>
       </c>
       <c r="I16" t="inlineStr"/>
     </row>
@@ -998,10 +998,10 @@
         <v>0.03547059004783595</v>
       </c>
       <c r="G17" t="n">
-        <v>0.05401775783592582</v>
+        <v>0.04604662814776475</v>
       </c>
       <c r="H17" t="n">
-        <v>52.28886173891385</v>
+        <v>29.8163579620916</v>
       </c>
       <c r="I17" t="inlineStr"/>
     </row>
@@ -1031,10 +1031,10 @@
         <v>0.1733142233776001</v>
       </c>
       <c r="G18" t="n">
-        <v>0.05058383807510915</v>
+        <v>0.108419126109293</v>
       </c>
       <c r="H18" t="n">
-        <v>-70.81379872389238</v>
+        <v>-37.44360734140095</v>
       </c>
       <c r="I18" t="inlineStr"/>
     </row>
@@ -1064,10 +1064,10 @@
         <v>0.1257529438542189</v>
       </c>
       <c r="G19" t="n">
-        <v>0.138707055639274</v>
+        <v>0.1647567187064278</v>
       </c>
       <c r="H19" t="n">
-        <v>10.30123938893419</v>
+        <v>31.01619227095363</v>
       </c>
       <c r="I19" t="inlineStr"/>
     </row>
@@ -1097,10 +1097,10 @@
         <v>0.1146520008062495</v>
       </c>
       <c r="G20" t="n">
-        <v>0.07182576877225617</v>
+        <v>0.05853392294243243</v>
       </c>
       <c r="H20" t="n">
-        <v>-37.35323564598354</v>
+        <v>-48.94644443113648</v>
       </c>
       <c r="I20" t="inlineStr"/>
     </row>
@@ -1130,10 +1130,10 @@
         <v>0.100398825941284</v>
       </c>
       <c r="G21" t="n">
-        <v>0.1237805203208007</v>
+        <v>0.1316067723317506</v>
       </c>
       <c r="H21" t="n">
-        <v>23.28881255363579</v>
+        <v>31.08397543285802</v>
       </c>
       <c r="I21" t="inlineStr"/>
     </row>
@@ -1163,10 +1163,10 @@
         <v>0.09419712915001806</v>
       </c>
       <c r="G22" t="n">
-        <v>0.08305949873652811</v>
+        <v>0.08567496814735316</v>
       </c>
       <c r="H22" t="n">
-        <v>-11.82374719271135</v>
+        <v>-9.04715576744651</v>
       </c>
       <c r="I22" t="inlineStr"/>
     </row>
@@ -1196,10 +1196,10 @@
         <v>0.1084899878672966</v>
       </c>
       <c r="G23" t="n">
-        <v>0.1148474650799891</v>
+        <v>0.1489898203414861</v>
       </c>
       <c r="H23" t="n">
-        <v>5.859966746856736</v>
+        <v>37.33047930996943</v>
       </c>
       <c r="I23" t="inlineStr"/>
     </row>
@@ -1229,10 +1229,10 @@
         <v>-0.1246243473874714</v>
       </c>
       <c r="G24" t="n">
-        <v>-0.246411992241941</v>
+        <v>-0.2345007264299186</v>
       </c>
       <c r="H24" t="n">
-        <v>97.72379748221897</v>
+        <v>-88.16606172534563</v>
       </c>
       <c r="I24" t="inlineStr"/>
     </row>
@@ -1262,10 +1262,10 @@
         <v>-0.2224540867233095</v>
       </c>
       <c r="G25" t="n">
-        <v>-0.2517363010620582</v>
+        <v>-0.2534370797270099</v>
       </c>
       <c r="H25" t="n">
-        <v>13.16326203310897</v>
+        <v>-13.92781470552949</v>
       </c>
       <c r="I25" t="inlineStr"/>
     </row>
@@ -1295,10 +1295,10 @@
         <v>0.1589818177106323</v>
       </c>
       <c r="G26" t="n">
-        <v>0.1708049136027349</v>
+        <v>0.1801779815692798</v>
       </c>
       <c r="H26" t="n">
-        <v>7.436759789488741</v>
+        <v>13.3324452845465</v>
       </c>
       <c r="I26" t="inlineStr"/>
     </row>
@@ -1328,10 +1328,10 @@
         <v>0.2004663364138392</v>
       </c>
       <c r="G27" t="n">
-        <v>0.1953350054754921</v>
+        <v>0.1895433507127082</v>
       </c>
       <c r="H27" t="n">
-        <v>-2.559697069414229</v>
+        <v>-5.44878800926545</v>
       </c>
       <c r="I27" t="inlineStr"/>
     </row>
@@ -1361,10 +1361,10 @@
         <v>-0.008030450210626818</v>
       </c>
       <c r="G28" t="n">
-        <v>0.00812330094678604</v>
+        <v>-0.00288365194142623</v>
       </c>
       <c r="H28" t="n">
-        <v>-201.1562332587076</v>
+        <v>64.09103019392053</v>
       </c>
       <c r="I28" t="inlineStr"/>
     </row>
@@ -1394,10 +1394,10 @@
         <v>0.0153774918446412</v>
       </c>
       <c r="G29" t="n">
-        <v>0.07388814226074111</v>
+        <v>0.01377899417678519</v>
       </c>
       <c r="H29" t="n">
-        <v>380.4954085310727</v>
+        <v>-10.3950480611899</v>
       </c>
       <c r="I29" t="inlineStr"/>
     </row>

</xml_diff>

<commit_message>
final grouped files updated
</commit_message>
<xml_diff>
--- a/Code/Data/DAX30/Compared Returns/Auto Recurrence/input 125/DAX30_returns_compared_annual.xlsx
+++ b/Code/Data/DAX30/Compared Returns/Auto Recurrence/input 125/DAX30_returns_compared_annual.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -53,18 +53,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -501,13 +501,13 @@
         <v>0.131420741763922</v>
       </c>
       <c r="G2" t="n">
-        <v>0.1811440960505368</v>
+        <v>0.1121418643933389</v>
       </c>
       <c r="H2" t="n">
-        <v>37.8352409362713</v>
+        <v>-14.66958496187364</v>
       </c>
       <c r="I2" t="n">
-        <v>3.460612640795781</v>
+        <v>7.354661273015827</v>
       </c>
     </row>
     <row r="3">
@@ -536,10 +536,10 @@
         <v>0.0890371962957979</v>
       </c>
       <c r="G3" t="n">
-        <v>0.1533243439897147</v>
+        <v>0.1698111566353668</v>
       </c>
       <c r="H3" t="n">
-        <v>72.20257416950002</v>
+        <v>90.71934393713722</v>
       </c>
       <c r="I3" t="inlineStr"/>
     </row>
@@ -569,10 +569,10 @@
         <v>-0.615343435918332</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.5924721202871878</v>
+        <v>-0.6541213138540207</v>
       </c>
       <c r="H4" t="n">
-        <v>3.71683750831132</v>
+        <v>-6.301826861582926</v>
       </c>
       <c r="I4" t="inlineStr"/>
     </row>
@@ -602,10 +602,10 @@
         <v>-0.6105932447668134</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.6530015889596703</v>
+        <v>-0.648846692997273</v>
       </c>
       <c r="H5" t="n">
-        <v>-6.945432914026537</v>
+        <v>-6.264964206256273</v>
       </c>
       <c r="I5" t="inlineStr"/>
     </row>
@@ -635,10 +635,10 @@
         <v>0.2461077835218171</v>
       </c>
       <c r="G6" t="n">
-        <v>0.2042452669095475</v>
+        <v>0.149913777806357</v>
       </c>
       <c r="H6" t="n">
-        <v>-17.00983041381889</v>
+        <v>-39.08612898743718</v>
       </c>
       <c r="I6" t="inlineStr"/>
     </row>
@@ -668,10 +668,10 @@
         <v>0.1638219427486889</v>
       </c>
       <c r="G7" t="n">
-        <v>0.3249686130804448</v>
+        <v>0.3285302406496415</v>
       </c>
       <c r="H7" t="n">
-        <v>98.36696331880461</v>
+        <v>100.5410478824704</v>
       </c>
       <c r="I7" t="inlineStr"/>
     </row>
@@ -701,10 +701,10 @@
         <v>0.165308928384769</v>
       </c>
       <c r="G8" t="n">
-        <v>0.1105988185832917</v>
+        <v>0.1186908439128481</v>
       </c>
       <c r="H8" t="n">
-        <v>-33.09567749065277</v>
+        <v>-28.20058476418997</v>
       </c>
       <c r="I8" t="inlineStr"/>
     </row>
@@ -734,10 +734,10 @@
         <v>0.1950925388973966</v>
       </c>
       <c r="G9" t="n">
-        <v>0.2142664248883905</v>
+        <v>0.2177951649834682</v>
       </c>
       <c r="H9" t="n">
-        <v>9.828098039709177</v>
+        <v>11.63684998636027</v>
       </c>
       <c r="I9" t="inlineStr"/>
     </row>
@@ -767,10 +767,10 @@
         <v>-0.05714634763265068</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.1245222012327999</v>
+        <v>-0.1289618669668079</v>
       </c>
       <c r="H10" t="n">
-        <v>-117.9005420140865</v>
+        <v>-125.66948249397</v>
       </c>
       <c r="I10" t="inlineStr"/>
     </row>
@@ -800,10 +800,10 @@
         <v>-0.1187683230189159</v>
       </c>
       <c r="G11" t="n">
-        <v>-0.1265913573149279</v>
+        <v>-0.1110998533787646</v>
       </c>
       <c r="H11" t="n">
-        <v>-6.58680201686947</v>
+        <v>6.456662387099604</v>
       </c>
       <c r="I11" t="inlineStr"/>
     </row>
@@ -833,10 +833,10 @@
         <v>0.1590292857940055</v>
       </c>
       <c r="G12" t="n">
-        <v>0.1850839586032318</v>
+        <v>0.1912955552428952</v>
       </c>
       <c r="H12" t="n">
-        <v>16.38356902575514</v>
+        <v>20.28951415318874</v>
       </c>
       <c r="I12" t="inlineStr"/>
     </row>
@@ -866,10 +866,10 @@
         <v>0.2056617473000462</v>
       </c>
       <c r="G13" t="n">
-        <v>0.2067866592343471</v>
+        <v>0.256380997536664</v>
       </c>
       <c r="H13" t="n">
-        <v>0.5469718842073983</v>
+        <v>24.66148951006526</v>
       </c>
       <c r="I13" t="inlineStr"/>
     </row>
@@ -899,10 +899,10 @@
         <v>0.1893730763108184</v>
       </c>
       <c r="G14" t="n">
-        <v>0.1750487029835016</v>
+        <v>0.230356093912151</v>
       </c>
       <c r="H14" t="n">
-        <v>-7.564102356243183</v>
+        <v>21.64141724881054</v>
       </c>
       <c r="I14" t="inlineStr"/>
     </row>
@@ -932,10 +932,10 @@
         <v>0.2499054176184599</v>
       </c>
       <c r="G15" t="n">
-        <v>0.2833445696460045</v>
+        <v>0.2276018980975815</v>
       </c>
       <c r="H15" t="n">
-        <v>13.38072313366068</v>
+        <v>-8.924784317773394</v>
       </c>
       <c r="I15" t="inlineStr"/>
     </row>
@@ -965,10 +965,10 @@
         <v>0.03648024689456582</v>
       </c>
       <c r="G16" t="n">
-        <v>0.05123395413793603</v>
+        <v>0.006153625119849877</v>
       </c>
       <c r="H16" t="n">
-        <v>40.44300271873422</v>
+        <v>-83.13162425233878</v>
       </c>
       <c r="I16" t="inlineStr"/>
     </row>
@@ -998,10 +998,10 @@
         <v>0.03547059004783595</v>
       </c>
       <c r="G17" t="n">
-        <v>0.04604662814776475</v>
+        <v>0.005021179681234354</v>
       </c>
       <c r="H17" t="n">
-        <v>29.8163579620916</v>
+        <v>-85.84410444127727</v>
       </c>
       <c r="I17" t="inlineStr"/>
     </row>
@@ -1031,10 +1031,10 @@
         <v>0.1733142233776001</v>
       </c>
       <c r="G18" t="n">
-        <v>0.108419126109293</v>
+        <v>0.08340672811650122</v>
       </c>
       <c r="H18" t="n">
-        <v>-37.44360734140095</v>
+        <v>-51.87542805717521</v>
       </c>
       <c r="I18" t="inlineStr"/>
     </row>
@@ -1064,10 +1064,10 @@
         <v>0.1257529438542189</v>
       </c>
       <c r="G19" t="n">
-        <v>0.1647567187064278</v>
+        <v>0.167108847032178</v>
       </c>
       <c r="H19" t="n">
-        <v>31.01619227095363</v>
+        <v>32.8866282652608</v>
       </c>
       <c r="I19" t="inlineStr"/>
     </row>
@@ -1097,10 +1097,10 @@
         <v>0.1146520008062495</v>
       </c>
       <c r="G20" t="n">
-        <v>0.05853392294243243</v>
+        <v>0.07762632544126712</v>
       </c>
       <c r="H20" t="n">
-        <v>-48.94644443113648</v>
+        <v>-32.29396356331548</v>
       </c>
       <c r="I20" t="inlineStr"/>
     </row>
@@ -1130,10 +1130,10 @@
         <v>0.100398825941284</v>
       </c>
       <c r="G21" t="n">
-        <v>0.1316067723317506</v>
+        <v>0.1377111428131169</v>
       </c>
       <c r="H21" t="n">
-        <v>31.08397543285802</v>
+        <v>37.16409681289914</v>
       </c>
       <c r="I21" t="inlineStr"/>
     </row>
@@ -1163,10 +1163,10 @@
         <v>0.09419712915001806</v>
       </c>
       <c r="G22" t="n">
-        <v>0.08567496814735316</v>
+        <v>0.10591232615147</v>
       </c>
       <c r="H22" t="n">
-        <v>-9.04715576744651</v>
+        <v>12.43689389173884</v>
       </c>
       <c r="I22" t="inlineStr"/>
     </row>
@@ -1196,10 +1196,10 @@
         <v>0.1084899878672966</v>
       </c>
       <c r="G23" t="n">
-        <v>0.1489898203414861</v>
+        <v>0.07934436199580493</v>
       </c>
       <c r="H23" t="n">
-        <v>37.33047930996943</v>
+        <v>-26.86480701531849</v>
       </c>
       <c r="I23" t="inlineStr"/>
     </row>
@@ -1229,10 +1229,10 @@
         <v>-0.1246243473874714</v>
       </c>
       <c r="G24" t="n">
-        <v>-0.2345007264299186</v>
+        <v>-0.1525691624515212</v>
       </c>
       <c r="H24" t="n">
-        <v>-88.16606172534563</v>
+        <v>-22.42323883724434</v>
       </c>
       <c r="I24" t="inlineStr"/>
     </row>
@@ -1262,10 +1262,10 @@
         <v>-0.2224540867233095</v>
       </c>
       <c r="G25" t="n">
-        <v>-0.2534370797270099</v>
+        <v>-0.2148527433246224</v>
       </c>
       <c r="H25" t="n">
-        <v>-13.92781470552949</v>
+        <v>3.417039223982303</v>
       </c>
       <c r="I25" t="inlineStr"/>
     </row>
@@ -1295,10 +1295,10 @@
         <v>0.1589818177106323</v>
       </c>
       <c r="G26" t="n">
-        <v>0.1801779815692798</v>
+        <v>0.1738512090749327</v>
       </c>
       <c r="H26" t="n">
-        <v>13.3324452845465</v>
+        <v>9.352888008466881</v>
       </c>
       <c r="I26" t="inlineStr"/>
     </row>
@@ -1328,10 +1328,10 @@
         <v>0.2004663364138392</v>
       </c>
       <c r="G27" t="n">
-        <v>0.1895433507127082</v>
+        <v>0.2074483805900574</v>
       </c>
       <c r="H27" t="n">
-        <v>-5.44878800926545</v>
+        <v>3.482901070135082</v>
       </c>
       <c r="I27" t="inlineStr"/>
     </row>
@@ -1361,10 +1361,10 @@
         <v>-0.008030450210626818</v>
       </c>
       <c r="G28" t="n">
-        <v>-0.00288365194142623</v>
+        <v>0.03557104591645446</v>
       </c>
       <c r="H28" t="n">
-        <v>64.09103019392053</v>
+        <v>542.9520759543811</v>
       </c>
       <c r="I28" t="inlineStr"/>
     </row>
@@ -1394,14 +1394,14 @@
         <v>0.0153774918446412</v>
       </c>
       <c r="G29" t="n">
-        <v>0.01377899417678519</v>
+        <v>-0.01232626068449046</v>
       </c>
       <c r="H29" t="n">
-        <v>-10.3950480611899</v>
+        <v>-180.1578099278001</v>
       </c>
       <c r="I29" t="inlineStr"/>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>